<commit_message>
v2.9: Globale Suche Fahrzeuge/Uebergabe, Ma.Ausdrucke + Krankmeldungen Sidebar, DokumentBrowser, Schaeden-Gesendet, Archiv-Funktion, Reparaturauftrag PDF
</commit_message>
<xml_diff>
--- a/Daten/Sonderaufgaben/Sonderaufgaben_2026_02_26.xlsx
+++ b/Daten/Sonderaufgaben/Sonderaufgaben_2026_02_26.xlsx
@@ -1295,13 +1295,13 @@
       <c r="B3" s="59" t="n"/>
       <c r="C3" s="55" t="inlineStr">
         <is>
-          <t>Mohammed</t>
+          <t>Yavgaan</t>
         </is>
       </c>
       <c r="D3" s="59" t="n"/>
       <c r="E3" s="55" t="inlineStr">
         <is>
-          <t>Hassainia</t>
+          <t>Timera</t>
         </is>
       </c>
       <c r="F3" s="59" t="n"/>
@@ -1316,7 +1316,7 @@
       <c r="B4" s="60" t="n"/>
       <c r="C4" s="55" t="inlineStr">
         <is>
-          <t>Oramba</t>
+          <t>Kalbfleisch</t>
         </is>
       </c>
       <c r="D4" s="59" t="n"/>
@@ -1350,7 +1350,7 @@
       <c r="B6" s="60" t="n"/>
       <c r="C6" s="16" t="inlineStr">
         <is>
-          <t>Bedl</t>
+          <t>Üzülmez</t>
         </is>
       </c>
       <c r="D6" s="60" t="n"/>
@@ -1377,7 +1377,7 @@
       <c r="D7" s="60" t="n"/>
       <c r="E7" s="32" t="inlineStr">
         <is>
-          <t>Su</t>
+          <t>Delgado</t>
         </is>
       </c>
       <c r="F7" s="64" t="n"/>
@@ -1392,13 +1392,13 @@
       <c r="B8" s="60" t="n"/>
       <c r="C8" s="16" t="inlineStr">
         <is>
-          <t>Etz / Idic / Etz</t>
+          <t>a.D</t>
         </is>
       </c>
       <c r="D8" s="60" t="n"/>
       <c r="E8" s="16" t="inlineStr">
         <is>
-          <t>a.D.</t>
+          <t>a.D</t>
         </is>
       </c>
       <c r="F8" s="60" t="n"/>
@@ -1419,7 +1419,7 @@
       <c r="D9" s="60" t="n"/>
       <c r="E9" s="32" t="inlineStr">
         <is>
-          <t>Rasch</t>
+          <t>Moeeni Mahvelati</t>
         </is>
       </c>
       <c r="F9" s="64" t="n"/>
@@ -1438,13 +1438,13 @@
       <c r="B10" s="60" t="n"/>
       <c r="C10" s="16" t="inlineStr">
         <is>
-          <t>Athanasiou</t>
+          <t>Idic</t>
         </is>
       </c>
       <c r="D10" s="60" t="n"/>
       <c r="E10" s="32" t="inlineStr">
         <is>
-          <t>Delgado</t>
+          <t>Rivola</t>
         </is>
       </c>
       <c r="F10" s="64" t="n"/>

</xml_diff>